<commit_message>
Adding red lights for when there is not enough resource
</commit_message>
<xml_diff>
--- a/18 Quintillion/Assets/Quintillion.xlsx
+++ b/18 Quintillion/Assets/Quintillion.xlsx
@@ -13,12 +13,11 @@
     <sheet name="quest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="380">
   <si>
     <t>"</t>
   </si>
@@ -1146,6 +1145,18 @@
   </si>
   <si>
     <t>The probe lands on a blue planet twinkling in the night, weaving its way down through a heavy mist which blankets weary land. Mighty shapes jut out everywhere, resistant to scans, advanced technology or unusual geology. Small bands of local inhabitants, shrouded in hooded woollen robes, emerge from the greyness and surround your probe. They whisper of a great bearded being who once passed through these lands speaking in sweeping terms of unimaginable bliss. With his words the traveler lured the youth of the local tribe with itself off towards much vaunted miracles at the galactic centre, though what those anointed secrets exactly were, no-one here clearly remembers. The locals present you with an ingredient of Hype: Being Wisely Economical with Information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   questTexts.Add("The probe lands on a blue planet twinkling in the night, weaving its way down through a heavy mist which blankets weary land. Mighty shapes jut out everywhere, resistant to scans, advanced technology or unusual geology. Small bands of local inhabitants, shrouded in hooded woollen robes, emerge from the greyness and surround your probe. They whisper of a great bearded being who once passed through these lands speaking in sweeping terms of unimaginable bliss. With his words the traveler lured the youth of the local tribe with itself off towards much vaunted miracles at the galactic centre, though what those anointed secrets exactly were, no-one here clearly remembers. The locals present you with an ingredient of Hype: Being Wisely Economical with Information.");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        questTexts.Add("The probe lands on a bustling communications station which is the meeting place of a thousand races; the last, best hope for peace; the nexus of this corner of the galaxy. The probe is wined and dined and you can share a hundred tales, true or false, from the worlds you have visited. You acquire a second ingredient of Hype: Good Connections, a Wink and a Nice Big Smile.");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        questTexts.Add("You land on a massive abandoned arkship. The probe can find no control room, no crew, merely doors that lead to other doors and corridors lined with strange mirrors wherein reanimated slivers of past lives, gilded memories of youth, a billion dreams of the future careen into each other in vivid colour and bewildering array. Highlights of life both fleshy and sublime. A miracle that even the probe with its miniscule brain struggles to leave behind. You acquire the third and final ingredient of Hype: The Drink Before and the Cigarette After are More Important than the Thing Itself. \nYou have acquired all the ingredients of Hype and can keep manufacturing it until Publication Day and beyond! And all with just one button - CONGRATULATIONS CLICKER.");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        engineNames1.Add("Wood");</t>
   </si>
 </sst>
 </file>
@@ -6560,10 +6571,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6586,6 +6597,26 @@
         <v>373</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>379</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tweaking purchase costs and polishing texts.
</commit_message>
<xml_diff>
--- a/18 Quintillion/Assets/Quintillion.xlsx
+++ b/18 Quintillion/Assets/Quintillion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12090" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12090" tabRatio="518"/>
   </bookViews>
   <sheets>
     <sheet name="worlds" sheetId="1" r:id="rId1"/>
@@ -256,18 +256,12 @@
     <t xml:space="preserve">partially covered by </t>
   </si>
   <si>
-    <t xml:space="preserve">sadly lacking any </t>
-  </si>
-  <si>
     <t xml:space="preserve">thoroughly permeated by </t>
   </si>
   <si>
     <t xml:space="preserve">soon to be famous for </t>
   </si>
   <si>
-    <t xml:space="preserve">welcoming us with </t>
-  </si>
-  <si>
     <t>part12</t>
   </si>
   <si>
@@ -283,18 +277,12 @@
     <t xml:space="preserve">levitating </t>
   </si>
   <si>
-    <t xml:space="preserve">hidden </t>
-  </si>
-  <si>
     <t xml:space="preserve">hypnotic </t>
   </si>
   <si>
     <t xml:space="preserve">pestilential </t>
   </si>
   <si>
-    <t xml:space="preserve">nourishing </t>
-  </si>
-  <si>
     <t xml:space="preserve">psychedelic </t>
   </si>
   <si>
@@ -331,9 +319,6 @@
     <t xml:space="preserve">intertwined with </t>
   </si>
   <si>
-    <t xml:space="preserve">and plenty of </t>
-  </si>
-  <si>
     <t xml:space="preserve">competing for space with </t>
   </si>
   <si>
@@ -481,9 +466,6 @@
     <t xml:space="preserve">ticklish </t>
   </si>
   <si>
-    <t xml:space="preserve">annoying </t>
-  </si>
-  <si>
     <t xml:space="preserve">two-faced </t>
   </si>
   <si>
@@ -505,9 +487,6 @@
     <t xml:space="preserve">feudal-capitalistic </t>
   </si>
   <si>
-    <t xml:space="preserve">extraordinarily civilised </t>
-  </si>
-  <si>
     <t xml:space="preserve">boulders </t>
   </si>
   <si>
@@ -616,9 +595,6 @@
     <t xml:space="preserve">who promise to grant our hearts' deepest desire, as long as that desire is for </t>
   </si>
   <si>
-    <t xml:space="preserve">to be much preferred over the </t>
-  </si>
-  <si>
     <t xml:space="preserve">bland, </t>
   </si>
   <si>
@@ -721,9 +697,6 @@
     <t xml:space="preserve">and the </t>
   </si>
   <si>
-    <t xml:space="preserve">not forgetting the </t>
-  </si>
-  <si>
     <t xml:space="preserve">topologically challenged </t>
   </si>
   <si>
@@ -748,9 +721,6 @@
     <t xml:space="preserve">chameleons </t>
   </si>
   <si>
-    <t xml:space="preserve">wallabies </t>
-  </si>
-  <si>
     <t xml:space="preserve">devils </t>
   </si>
   <si>
@@ -760,9 +730,6 @@
     <t xml:space="preserve">pidgeons </t>
   </si>
   <si>
-    <t xml:space="preserve">who can be found always gleefully pestering the </t>
-  </si>
-  <si>
     <t xml:space="preserve">about to make us so very happy once we lay hands on its untouched reserves of </t>
   </si>
   <si>
@@ -961,9 +928,6 @@
     <t xml:space="preserve">shrubberies </t>
   </si>
   <si>
-    <t xml:space="preserve">which form the primary sustenance of the native, memorably </t>
-  </si>
-  <si>
     <t xml:space="preserve">which provide shelter for the indigenous </t>
   </si>
   <si>
@@ -973,18 +937,12 @@
     <t xml:space="preserve">curiously heptagonal </t>
   </si>
   <si>
-    <t xml:space="preserve">who exist in a wary truce with the world's apex predators, the  </t>
-  </si>
-  <si>
     <t xml:space="preserve">melodious </t>
   </si>
   <si>
     <t>dolphinoids</t>
   </si>
   <si>
-    <t>annelids</t>
-  </si>
-  <si>
     <t>pasta-shapes</t>
   </si>
   <si>
@@ -1003,9 +961,6 @@
     <t>octopuses</t>
   </si>
   <si>
-    <t>sticks</t>
-  </si>
-  <si>
     <t>trombones</t>
   </si>
   <si>
@@ -1060,9 +1015,6 @@
     <t xml:space="preserve">stand-up comedians </t>
   </si>
   <si>
-    <t xml:space="preserve">simple, cooperative and ultimately rather pathetic </t>
-  </si>
-  <si>
     <t xml:space="preserve">eye-poppingly </t>
   </si>
   <si>
@@ -1129,12 +1081,6 @@
     <t xml:space="preserve">who will give us their wealth, sure, but insist that we also take their </t>
   </si>
   <si>
-    <t xml:space="preserve">whose lives are entirely structured around the tragic mediocrity of one day writing "good characters", and using the projected moderate literary fame coming from this to acquire some of the galactic region's </t>
-  </si>
-  <si>
-    <t xml:space="preserve">whose elders present to us their </t>
-  </si>
-  <si>
     <t xml:space="preserve">(probably) fermentable </t>
   </si>
   <si>
@@ -1157,6 +1103,60 @@
   </si>
   <si>
     <t xml:space="preserve">        engineNames1.Add("Wood");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adorned by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crammed to the brim with  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">politically astute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">evaginated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">emitting beeps when found near </t>
+  </si>
+  <si>
+    <t xml:space="preserve">which form the primary sustenance of the roaming </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sturgeons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">second on this world only to the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">who exist in a wary truce with the world's apex predators, some </t>
+  </si>
+  <si>
+    <t xml:space="preserve">who are frankly no better dinner company than the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">who are often found gleefully pestering the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">magnetic </t>
+  </si>
+  <si>
+    <t>genital warts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">practically celibate </t>
+  </si>
+  <si>
+    <t>nano-sticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deeply contemplative </t>
+  </si>
+  <si>
+    <t xml:space="preserve">whose elders solemnly present to us their </t>
+  </si>
+  <si>
+    <t xml:space="preserve">whose lives are entirely structured around the tragic mediocrity of writing stories, and using the projected moderate literary fame coming from this to acquire some of the galactic region's </t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G340"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="B317" sqref="B317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1544,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1559,7 +1559,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1604,7 +1604,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -1814,7 +1814,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1919,7 +1919,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
@@ -1934,7 +1934,7 @@
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -1979,14 +1979,14 @@
         <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="str">
-        <f>A34&amp;".Add("&amp;C34&amp;G37&amp;C34&amp;");"</f>
-        <v>part4.Add("");</v>
+        <f t="shared" si="4"/>
+        <v>part4.Add("suspect, ");</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -2086,7 +2086,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -2101,7 +2101,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -2176,7 +2176,7 @@
         <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
@@ -2221,7 +2221,7 @@
         <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
@@ -2293,7 +2293,7 @@
         <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
@@ -2578,7 +2578,7 @@
         <v>47</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
@@ -2593,7 +2593,7 @@
         <v>47</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
@@ -2608,7 +2608,7 @@
         <v>47</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="C80" t="s">
         <v>0</v>
@@ -2698,7 +2698,7 @@
         <v>47</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>48</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
@@ -2728,7 +2728,7 @@
         <v>48</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
@@ -2743,7 +2743,7 @@
         <v>48</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
@@ -2758,7 +2758,7 @@
         <v>48</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
@@ -2773,7 +2773,7 @@
         <v>48</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
         <v>48</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C93" t="s">
         <v>0</v>
@@ -2803,7 +2803,7 @@
         <v>48</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s">
         <v>0</v>
@@ -2818,7 +2818,7 @@
         <v>48</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
@@ -2833,7 +2833,7 @@
         <v>48</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
@@ -2848,7 +2848,7 @@
         <v>48</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
@@ -2998,7 +2998,7 @@
         <v>64</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C108" t="s">
         <v>0</v>
@@ -3013,7 +3013,7 @@
         <v>65</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C110" t="s">
         <v>0</v>
@@ -3058,7 +3058,7 @@
         <v>65</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C113" t="s">
         <v>0</v>
@@ -3103,14 +3103,14 @@
         <v>65</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>79</v>
+        <v>362</v>
       </c>
       <c r="C116" t="s">
         <v>0</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="13"/>
-        <v>part11.Add("sadly lacking any ");</v>
+        <v>part11.Add("adorned by ");</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>65</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C117" t="s">
         <v>0</v>
@@ -3133,7 +3133,7 @@
         <v>65</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C118" t="s">
         <v>0</v>
@@ -3148,22 +3148,22 @@
         <v>65</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>82</v>
+        <v>363</v>
       </c>
       <c r="C119" t="s">
         <v>0</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="13"/>
-        <v>part11.Add("welcoming us with ");</v>
+        <v>part11.Add("crammed to the brim with  ");</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C121" t="s">
         <v>0</v>
@@ -3175,25 +3175,25 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>88</v>
+        <v>365</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="14"/>
-        <v>part12.Add("hidden ");</v>
+        <v>part12.Add("evaginated ");</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C123" t="s">
         <v>0</v>
@@ -3205,10 +3205,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>81</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C124" t="s">
         <v>0</v>
@@ -3220,10 +3220,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C125" t="s">
         <v>0</v>
@@ -3235,10 +3235,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C126" t="s">
         <v>0</v>
@@ -3250,10 +3250,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C127" t="s">
         <v>0</v>
@@ -3265,25 +3265,25 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>91</v>
+        <v>364</v>
       </c>
       <c r="C128" t="s">
         <v>0</v>
       </c>
       <c r="D128" t="str">
         <f t="shared" si="14"/>
-        <v>part12.Add("nourishing ");</v>
+        <v>part12.Add("politically astute ");</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C129" t="s">
         <v>0</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C130" t="s">
         <v>0</v>
@@ -3310,10 +3310,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C132" t="s">
         <v>0</v>
@@ -3325,10 +3325,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C133" t="s">
         <v>0</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C134" t="s">
         <v>0</v>
@@ -3355,10 +3355,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C135" t="s">
         <v>0</v>
@@ -3370,10 +3370,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C136" t="s">
         <v>0</v>
@@ -3385,10 +3385,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C137" t="s">
         <v>0</v>
@@ -3400,10 +3400,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C138" t="s">
         <v>0</v>
@@ -3415,10 +3415,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C139" t="s">
         <v>0</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C140" t="s">
         <v>0</v>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C141" t="s">
         <v>0</v>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C143" t="s">
         <v>0</v>
@@ -3475,10 +3475,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C144" t="s">
         <v>0</v>
@@ -3490,10 +3490,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C145" t="s">
         <v>0</v>
@@ -3505,10 +3505,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C146" t="s">
         <v>0</v>
@@ -3520,10 +3520,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C147" t="s">
         <v>0</v>
@@ -3535,10 +3535,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C148" t="s">
         <v>0</v>
@@ -3550,10 +3550,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C149" t="s">
         <v>0</v>
@@ -3565,25 +3565,25 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>104</v>
+        <v>366</v>
       </c>
       <c r="C150" t="s">
         <v>0</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="16"/>
-        <v>part14.Add("and plenty of ");</v>
+        <v>part14.Add("emitting beeps when found near ");</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C151" t="s">
         <v>0</v>
@@ -3595,10 +3595,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C152" t="s">
         <v>0</v>
@@ -3610,10 +3610,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="C154" t="s">
         <v>0</v>
@@ -3625,10 +3625,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C155" t="s">
         <v>0</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C156" t="s">
         <v>0</v>
@@ -3655,10 +3655,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C157" t="s">
         <v>0</v>
@@ -3670,10 +3670,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C158" t="s">
         <v>0</v>
@@ -3685,10 +3685,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C159" t="s">
         <v>0</v>
@@ -3700,10 +3700,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C160" t="s">
         <v>0</v>
@@ -3715,10 +3715,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C161" t="s">
         <v>0</v>
@@ -3730,10 +3730,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C162" t="s">
         <v>0</v>
@@ -3745,10 +3745,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C163" t="s">
         <v>0</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="C165" t="s">
         <v>0</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C166" t="s">
         <v>0</v>
@@ -3790,10 +3790,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C167" t="s">
         <v>0</v>
@@ -3805,10 +3805,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C168" t="s">
         <v>0</v>
@@ -3820,10 +3820,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C169" t="s">
         <v>0</v>
@@ -3835,10 +3835,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C170" t="s">
         <v>0</v>
@@ -3850,10 +3850,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C171" t="s">
         <v>0</v>
@@ -3865,10 +3865,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C172" t="s">
         <v>0</v>
@@ -3880,10 +3880,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C173" t="s">
         <v>0</v>
@@ -3895,10 +3895,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C174" t="s">
         <v>0</v>
@@ -3910,25 +3910,25 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
       <c r="C176" t="s">
         <v>0</v>
       </c>
       <c r="D176" t="str">
         <f t="shared" ref="D176:D185" si="19">A176&amp;".Add("&amp;C176&amp;B176&amp;C176&amp;");"</f>
-        <v>part17.Add("which form the primary sustenance of the native, memorably ");</v>
+        <v>part17.Add("which form the primary sustenance of the roaming ");</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C177" t="s">
         <v>0</v>
@@ -3940,10 +3940,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C178" t="s">
         <v>0</v>
@@ -3955,10 +3955,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C179" t="s">
         <v>0</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="C180" t="s">
         <v>0</v>
@@ -3985,10 +3985,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C181" t="s">
         <v>0</v>
@@ -4000,10 +4000,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C182" t="s">
         <v>0</v>
@@ -4015,10 +4015,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C183" t="s">
         <v>0</v>
@@ -4030,10 +4030,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C184" t="s">
         <v>0</v>
@@ -4045,10 +4045,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C185" t="s">
         <v>0</v>
@@ -4060,10 +4060,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C187" t="s">
         <v>0</v>
@@ -4075,10 +4075,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C188" t="s">
         <v>0</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C189" t="s">
         <v>0</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" t="s">
@@ -4118,10 +4118,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>114</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C191" t="s">
         <v>0</v>
@@ -4133,10 +4133,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C192" t="s">
         <v>0</v>
@@ -4148,10 +4148,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C193" t="s">
         <v>0</v>
@@ -4163,10 +4163,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C194" t="s">
         <v>0</v>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C195" t="s">
         <v>0</v>
@@ -4193,10 +4193,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C196" t="s">
         <v>0</v>
@@ -4208,10 +4208,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C198" t="s">
         <v>0</v>
@@ -4223,10 +4223,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C199" t="s">
         <v>0</v>
@@ -4238,10 +4238,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C200" t="s">
         <v>0</v>
@@ -4253,10 +4253,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C201" t="s">
         <v>0</v>
@@ -4268,10 +4268,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C202" t="s">
         <v>0</v>
@@ -4283,10 +4283,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C203" t="s">
         <v>0</v>
@@ -4298,10 +4298,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="C204" t="s">
         <v>0</v>
@@ -4313,10 +4313,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C205" t="s">
         <v>0</v>
@@ -4328,10 +4328,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C206" t="s">
         <v>0</v>
@@ -4343,10 +4343,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C207" t="s">
         <v>0</v>
@@ -4358,10 +4358,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C209" t="s">
         <v>0</v>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C210" t="s">
         <v>0</v>
@@ -4388,10 +4388,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C211" t="s">
         <v>0</v>
@@ -4403,10 +4403,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C212" t="s">
         <v>0</v>
@@ -4418,10 +4418,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>132</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="C213" t="s">
         <v>0</v>
@@ -4433,10 +4433,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C214" t="s">
         <v>0</v>
@@ -4448,10 +4448,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C215" t="s">
         <v>0</v>
@@ -4463,10 +4463,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C216" t="s">
         <v>0</v>
@@ -4478,10 +4478,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C217" t="s">
         <v>0</v>
@@ -4493,10 +4493,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C218" t="s">
         <v>0</v>
@@ -4508,10 +4508,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B220" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C220" t="s">
         <v>0</v>
@@ -4523,10 +4523,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B221" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C221" t="s">
         <v>0</v>
@@ -4538,10 +4538,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B222" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C222" t="s">
         <v>0</v>
@@ -4553,10 +4553,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B223" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C223" t="s">
         <v>0</v>
@@ -4568,10 +4568,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B224" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C224" t="s">
         <v>0</v>
@@ -4583,10 +4583,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B225" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C225" t="s">
         <v>0</v>
@@ -4598,25 +4598,25 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B226" t="s">
-        <v>243</v>
+        <v>368</v>
       </c>
       <c r="C226" t="s">
         <v>0</v>
       </c>
       <c r="D226" t="str">
         <f t="shared" si="23"/>
-        <v>part21.Add("wallabies ");</v>
+        <v>part21.Add("sturgeons ");</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B227" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C227" t="s">
         <v>0</v>
@@ -4628,10 +4628,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B228" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C228" t="s">
         <v>0</v>
@@ -4643,10 +4643,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C229" t="s">
         <v>0</v>
@@ -4658,55 +4658,55 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B231" t="s">
-        <v>234</v>
+        <v>369</v>
       </c>
       <c r="C231" t="s">
         <v>0</v>
       </c>
       <c r="D231" t="str">
         <f t="shared" ref="D231:D240" si="24">A231&amp;".Add("&amp;C231&amp;B231&amp;C231&amp;");"</f>
-        <v>part22.Add("not forgetting the ");</v>
+        <v>part22.Add("second on this world only to the ");</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B232" t="s">
-        <v>318</v>
+        <v>370</v>
       </c>
       <c r="C232" t="s">
         <v>0</v>
       </c>
       <c r="D232" t="str">
         <f t="shared" si="24"/>
-        <v>part22.Add("who exist in a wary truce with the world's apex predators, the  ");</v>
+        <v>part22.Add("who exist in a wary truce with the world's apex predators, some ");</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B233" t="s">
-        <v>199</v>
+        <v>371</v>
       </c>
       <c r="C233" t="s">
         <v>0</v>
       </c>
       <c r="D233" t="str">
         <f t="shared" si="24"/>
-        <v>part22.Add("to be much preferred over the ");</v>
+        <v>part22.Add("who are frankly no better dinner company than the ");</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B234" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C234" t="s">
         <v>0</v>
@@ -4718,10 +4718,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B235" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C235" t="s">
         <v>0</v>
@@ -4733,25 +4733,25 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>372</v>
       </c>
       <c r="C236" t="s">
         <v>0</v>
       </c>
       <c r="D236" t="str">
         <f t="shared" si="24"/>
-        <v>part22.Add("who can be found always gleefully pestering the ");</v>
+        <v>part22.Add("who are often found gleefully pestering the ");</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C237" t="s">
         <v>0</v>
@@ -4763,10 +4763,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B238" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C238" t="s">
         <v>0</v>
@@ -4778,10 +4778,10 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B239" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C239" t="s">
         <v>0</v>
@@ -4793,10 +4793,10 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B240" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C240" t="s">
         <v>0</v>
@@ -4808,10 +4808,10 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B242" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C242" t="s">
         <v>0</v>
@@ -4823,10 +4823,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B243" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C243" t="s">
         <v>0</v>
@@ -4838,10 +4838,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B244" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C244" t="s">
         <v>0</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B245" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C245" t="s">
         <v>0</v>
@@ -4868,10 +4868,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B246" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C246" t="s">
         <v>0</v>
@@ -4883,10 +4883,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B247" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C247" t="s">
         <v>0</v>
@@ -4898,25 +4898,25 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B248" t="s">
-        <v>154</v>
+        <v>373</v>
       </c>
       <c r="C248" t="s">
         <v>0</v>
       </c>
       <c r="D248" t="str">
         <f t="shared" si="25"/>
-        <v>part23.Add("annoying ");</v>
+        <v>part23.Add("magnetic ");</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B249" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C249" t="s">
         <v>0</v>
@@ -4928,10 +4928,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B250" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C250" t="s">
         <v>0</v>
@@ -4943,10 +4943,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B251" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C251" t="s">
         <v>0</v>
@@ -4958,10 +4958,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B253" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="C253" t="s">
         <v>0</v>
@@ -4973,25 +4973,25 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B254" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="C254" t="s">
         <v>0</v>
       </c>
       <c r="D254" t="str">
         <f t="shared" si="26"/>
-        <v>part24.Add("annelids");</v>
+        <v>part24.Add("genital warts");</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="C255" t="s">
         <v>0</v>
@@ -5003,10 +5003,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C256" t="s">
         <v>0</v>
@@ -5018,10 +5018,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C257" t="s">
         <v>0</v>
@@ -5033,10 +5033,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C258" t="s">
         <v>0</v>
@@ -5048,10 +5048,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="C259" t="s">
         <v>0</v>
@@ -5063,10 +5063,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="C260" t="s">
         <v>0</v>
@@ -5078,25 +5078,25 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>328</v>
+        <v>376</v>
       </c>
       <c r="C261" t="s">
         <v>0</v>
       </c>
       <c r="D261" t="str">
         <f t="shared" si="26"/>
-        <v>part24.Add("sticks");</v>
+        <v>part24.Add("nano-sticks");</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C262" t="s">
         <v>0</v>
@@ -5108,10 +5108,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B264" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C264" t="s">
         <v>0</v>
@@ -5123,10 +5123,10 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B265" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C265" t="s">
         <v>0</v>
@@ -5138,10 +5138,10 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C266" t="s">
         <v>0</v>
@@ -5153,10 +5153,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C267" t="s">
         <v>0</v>
@@ -5168,10 +5168,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C268" t="s">
         <v>0</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C269" t="s">
         <v>0</v>
@@ -5198,10 +5198,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C270" t="s">
         <v>0</v>
@@ -5213,10 +5213,10 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C271" t="s">
         <v>0</v>
@@ -5228,10 +5228,10 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="C272" t="s">
         <v>0</v>
@@ -5243,10 +5243,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C273" t="s">
         <v>0</v>
@@ -5258,10 +5258,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B275" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C275" t="s">
         <v>0</v>
@@ -5273,10 +5273,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B276" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C276" t="s">
         <v>0</v>
@@ -5288,10 +5288,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B277" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C277" t="s">
         <v>0</v>
@@ -5303,40 +5303,40 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B278" t="s">
-        <v>347</v>
+        <v>377</v>
       </c>
       <c r="C278" t="s">
         <v>0</v>
       </c>
       <c r="D278" t="str">
         <f t="shared" si="28"/>
-        <v>part26.Add("simple, cooperative and ultimately rather pathetic ");</v>
+        <v>part26.Add("deeply contemplative ");</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B279" t="s">
-        <v>162</v>
+        <v>375</v>
       </c>
       <c r="C279" t="s">
         <v>0</v>
       </c>
       <c r="D279" t="str">
         <f t="shared" si="28"/>
-        <v>part26.Add("extraordinarily civilised ");</v>
+        <v>part26.Add("practically celibate ");</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B280" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C280" t="s">
         <v>0</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B281" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C281" t="s">
         <v>0</v>
@@ -5363,10 +5363,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B282" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C282" t="s">
         <v>0</v>
@@ -5378,10 +5378,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B283" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C283" t="s">
         <v>0</v>
@@ -5393,10 +5393,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B284" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="C284" t="s">
         <v>0</v>
@@ -5408,10 +5408,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B286" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C286" t="s">
         <v>0</v>
@@ -5423,10 +5423,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B287" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C287" t="s">
         <v>0</v>
@@ -5438,10 +5438,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B288" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C288" t="s">
         <v>0</v>
@@ -5453,10 +5453,10 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B289" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C289" t="s">
         <v>0</v>
@@ -5468,10 +5468,10 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B290" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C290" t="s">
         <v>0</v>
@@ -5483,10 +5483,10 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B291" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C291" t="s">
         <v>0</v>
@@ -5498,10 +5498,10 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B292" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C292" t="s">
         <v>0</v>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B293" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C293" t="s">
         <v>0</v>
@@ -5528,10 +5528,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B294" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C294" t="s">
         <v>0</v>
@@ -5543,10 +5543,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B295" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C295" t="s">
         <v>0</v>
@@ -5558,10 +5558,10 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B297" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C297" t="s">
         <v>0</v>
@@ -5573,10 +5573,10 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B298" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C298" t="s">
         <v>0</v>
@@ -5588,10 +5588,10 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B299" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C299" t="s">
         <v>0</v>
@@ -5603,10 +5603,10 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B300" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="C300" t="s">
         <v>0</v>
@@ -5618,25 +5618,25 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B301" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C301" t="s">
         <v>0</v>
       </c>
       <c r="D301" t="str">
         <f t="shared" si="30"/>
-        <v>part28.Add("whose elders present to us their ");</v>
+        <v>part28.Add("whose elders solemnly present to us their ");</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B302" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C302" t="s">
         <v>0</v>
@@ -5648,10 +5648,10 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B303" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C303" t="s">
         <v>0</v>
@@ -5663,10 +5663,10 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B304" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C304" t="s">
         <v>0</v>
@@ -5678,10 +5678,10 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B305" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C305" t="s">
         <v>0</v>
@@ -5693,10 +5693,10 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B306" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C306" t="s">
         <v>0</v>
@@ -5708,10 +5708,10 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B308" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C308" t="s">
         <v>0</v>
@@ -5723,10 +5723,10 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B309" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="C309" t="s">
         <v>0</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B310" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="C310" t="s">
         <v>0</v>
@@ -5753,10 +5753,10 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B311" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="C311" t="s">
         <v>0</v>
@@ -5768,10 +5768,10 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B312" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="C312" t="s">
         <v>0</v>
@@ -5783,10 +5783,10 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B313" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="C313" t="s">
         <v>0</v>
@@ -5798,10 +5798,10 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B314" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="C314" t="s">
         <v>0</v>
@@ -5813,10 +5813,10 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B315" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C315" t="s">
         <v>0</v>
@@ -5828,10 +5828,10 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B316" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="C316" t="s">
         <v>0</v>
@@ -5841,27 +5841,27 @@
         <v>part29.Add("who will give us their wealth, sure, but insist that we also take their ");</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="C317" t="s">
         <v>0</v>
       </c>
       <c r="D317" t="str">
         <f t="shared" si="31"/>
-        <v>part29.Add("whose lives are entirely structured around the tragic mediocrity of one day writing "good characters", and using the projected moderate literary fame coming from this to acquire some of the galactic region's ");</v>
+        <v>part29.Add("whose lives are entirely structured around the tragic mediocrity of writing stories, and using the projected moderate literary fame coming from this to acquire some of the galactic region's ");</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B319" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C319" t="s">
         <v>0</v>
@@ -5873,10 +5873,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B320" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C320" t="s">
         <v>0</v>
@@ -5888,10 +5888,10 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B321" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C321" t="s">
         <v>0</v>
@@ -5903,10 +5903,10 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B322" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C322" t="s">
         <v>0</v>
@@ -5918,10 +5918,10 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B323" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C323" t="s">
         <v>0</v>
@@ -5933,10 +5933,10 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
+        <v>168</v>
+      </c>
+      <c r="B324" t="s">
         <v>175</v>
-      </c>
-      <c r="B324" t="s">
-        <v>182</v>
       </c>
       <c r="C324" t="s">
         <v>0</v>
@@ -5948,10 +5948,10 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B325" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C325" t="s">
         <v>0</v>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B326" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C326" t="s">
         <v>0</v>
@@ -5978,10 +5978,10 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B327" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C327" t="s">
         <v>0</v>
@@ -5993,10 +5993,10 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B328" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C328" t="s">
         <v>0</v>
@@ -6008,10 +6008,10 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B331" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="C331" t="s">
         <v>0</v>
@@ -6023,10 +6023,10 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B332" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="C332" t="s">
         <v>0</v>
@@ -6038,10 +6038,10 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B333" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="C333" t="s">
         <v>0</v>
@@ -6053,10 +6053,10 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B334" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="C334" t="s">
         <v>0</v>
@@ -6068,10 +6068,10 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B335" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="C335" t="s">
         <v>0</v>
@@ -6083,10 +6083,10 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B336" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="C336" t="s">
         <v>0</v>
@@ -6098,10 +6098,10 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B337" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C337" t="s">
         <v>0</v>
@@ -6113,10 +6113,10 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B338" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="C338" t="s">
         <v>0</v>
@@ -6128,10 +6128,10 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B339" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="C339" t="s">
         <v>0</v>
@@ -6143,10 +6143,10 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B340" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="C340" t="s">
         <v>0</v>
@@ -6179,21 +6179,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" t="s">
         <v>268</v>
-      </c>
-      <c r="B2" t="s">
-        <v>279</v>
       </c>
       <c r="C2" t="str">
         <f>$A$1&amp;".Add("&amp;E2&amp;A2&amp;E2&amp;");"</f>
@@ -6209,10 +6209,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C11" si="0">$A$1&amp;".Add("&amp;E3&amp;A3&amp;E3&amp;");"</f>
@@ -6228,10 +6228,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -6247,10 +6247,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -6266,10 +6266,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" t="s">
         <v>272</v>
-      </c>
-      <c r="B6" t="s">
-        <v>283</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -6285,10 +6285,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7" t="s">
         <v>274</v>
-      </c>
-      <c r="B7" t="s">
-        <v>285</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -6304,10 +6304,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -6323,10 +6323,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -6342,10 +6342,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -6361,10 +6361,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -6401,10 +6401,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C1" t="str">
         <f t="shared" ref="C1:C10" si="0">B$1&amp;".Add("&amp;D1&amp;A1&amp;D1&amp;");"</f>
@@ -6416,10 +6416,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
@@ -6431,10 +6431,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -6446,10 +6446,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -6461,10 +6461,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -6476,10 +6476,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -6491,10 +6491,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -6506,10 +6506,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B8" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -6521,10 +6521,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -6536,10 +6536,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -6551,10 +6551,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B11" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11" si="1">B$1&amp;".Add("&amp;D11&amp;A11&amp;D11&amp;");"</f>
@@ -6573,8 +6573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6584,37 +6584,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More music, polished texts, fixed bugs
</commit_message>
<xml_diff>
--- a/18 Quintillion/Assets/Quintillion.xlsx
+++ b/18 Quintillion/Assets/Quintillion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12090" tabRatio="518"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12090" tabRatio="518" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="worlds" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="381">
   <si>
     <t>"</t>
   </si>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">entirely </t>
   </si>
   <si>
-    <t xml:space="preserve">partly </t>
-  </si>
-  <si>
     <t>part3</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t xml:space="preserve">artefact </t>
   </si>
   <si>
-    <t xml:space="preserve">ring </t>
-  </si>
-  <si>
     <t xml:space="preserve">space turtle </t>
   </si>
   <si>
@@ -235,9 +229,6 @@
     <t xml:space="preserve">its jungles </t>
   </si>
   <si>
-    <t xml:space="preserve">its arctic zones </t>
-  </si>
-  <si>
     <t xml:space="preserve">its surface </t>
   </si>
   <si>
@@ -619,9 +610,6 @@
     <t xml:space="preserve">who are practically begging us to lift them to the stars in exchange for their </t>
   </si>
   <si>
-    <t xml:space="preserve">who may be swiftly swindled of their </t>
-  </si>
-  <si>
     <t xml:space="preserve">delightfully </t>
   </si>
   <si>
@@ -676,9 +664,6 @@
     <t xml:space="preserve">giving sustenance to the </t>
   </si>
   <si>
-    <t xml:space="preserve">excreted on by the </t>
-  </si>
-  <si>
     <t xml:space="preserve">jealously guarded by </t>
   </si>
   <si>
@@ -745,9 +730,6 @@
     <t xml:space="preserve">who vigorously pellet the probe with their </t>
   </si>
   <si>
-    <t xml:space="preserve">who seem quite happy to trade us their </t>
-  </si>
-  <si>
     <t xml:space="preserve">game developers </t>
   </si>
   <si>
@@ -934,9 +916,6 @@
     <t xml:space="preserve">providing protected habitats for the local </t>
   </si>
   <si>
-    <t xml:space="preserve">curiously heptagonal </t>
-  </si>
-  <si>
     <t xml:space="preserve">melodious </t>
   </si>
   <si>
@@ -979,12 +958,6 @@
     <t xml:space="preserve"> dwelling in the ruined complexes of </t>
   </si>
   <si>
-    <t xml:space="preserve">. These beings are projected to evolve into </t>
-  </si>
-  <si>
-    <t xml:space="preserve">. In barely comprehensible ways these creatures are pleading to become </t>
-  </si>
-  <si>
     <t xml:space="preserve"> who have been domesticated by a civilisation of </t>
   </si>
   <si>
@@ -1054,9 +1027,6 @@
     <t xml:space="preserve">gentle cuticle treatments. </t>
   </si>
   <si>
-    <t xml:space="preserve">foul-smelling but addictive ointment. </t>
-  </si>
-  <si>
     <t xml:space="preserve">perverted, </t>
   </si>
   <si>
@@ -1157,6 +1127,39 @@
   </si>
   <si>
     <t xml:space="preserve">whose lives are entirely structured around the tragic mediocrity of writing stories, and using the projected moderate literary fame coming from this to acquire some of the galactic region's </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. These beings, who are actually the smartest things on the world, are typically worn as hats by the local, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">. These curious creatures are being ruthlessly slaughtered towards extinction by a roaming horde of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">who themselves seem quite happy to trade us their </t>
+  </si>
+  <si>
+    <t xml:space="preserve">who, might I suggest, may be swiftly swindled of their </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heptagonally gendered </t>
+  </si>
+  <si>
+    <t xml:space="preserve">furiously excreted on by the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">its lofty peaks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ringworld </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mind-crushingly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">foul-smelling but addictive herbal ointment. </t>
+  </si>
+  <si>
+    <t>Hmm, the camera is not working. Close your eyes and wish upon a star?</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="B317" sqref="B317"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D340" sqref="D1:D340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1559,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1574,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1604,7 +1607,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1634,14 +1637,14 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>378</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>part1.Add("partly ");</v>
+        <v>part1.Add("mind-crushingly ");</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -1664,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -1679,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -1694,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -1709,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -1724,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1739,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -1754,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -1769,7 +1772,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -1784,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1799,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -1811,10 +1814,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1826,10 +1829,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -1841,10 +1844,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
@@ -1856,10 +1859,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -1871,10 +1874,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
@@ -1886,10 +1889,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
@@ -1901,10 +1904,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
@@ -1916,10 +1919,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
@@ -1931,10 +1934,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -1946,10 +1949,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -1961,10 +1964,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -1976,10 +1979,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -1991,10 +1994,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
@@ -2006,10 +2009,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
@@ -2022,10 +2025,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
@@ -2037,10 +2040,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
@@ -2052,10 +2055,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
@@ -2068,10 +2071,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -2083,10 +2086,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -2098,10 +2101,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -2113,10 +2116,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" t="s">
-        <v>24</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
@@ -2128,10 +2131,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
@@ -2143,10 +2146,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
@@ -2158,10 +2161,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
         <v>0</v>
@@ -2173,10 +2176,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
@@ -2188,10 +2191,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
@@ -2203,10 +2206,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
@@ -2218,10 +2221,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
@@ -2233,10 +2236,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
@@ -2248,7 +2251,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
@@ -2260,10 +2263,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
@@ -2275,10 +2278,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
@@ -2290,10 +2293,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
@@ -2305,10 +2308,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
@@ -2320,10 +2323,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
@@ -2335,10 +2338,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
@@ -2350,10 +2353,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
@@ -2365,10 +2368,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
@@ -2380,10 +2383,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
@@ -2395,10 +2398,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
@@ -2410,10 +2413,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C66" t="s">
         <v>0</v>
@@ -2425,10 +2428,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
@@ -2440,10 +2443,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
@@ -2455,10 +2458,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
@@ -2470,10 +2473,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
@@ -2485,10 +2488,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
@@ -2500,10 +2503,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C72" t="s">
         <v>0</v>
@@ -2515,10 +2518,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C73" t="s">
         <v>0</v>
@@ -2530,25 +2533,25 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>52</v>
+        <v>377</v>
       </c>
       <c r="C74" t="s">
         <v>0</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="9"/>
-        <v>part7.Add("ring ");</v>
+        <v>part7.Add("ringworld ");</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
         <v>0</v>
@@ -2560,10 +2563,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
@@ -2575,10 +2578,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
@@ -2590,10 +2593,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
@@ -2605,10 +2608,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C80" t="s">
         <v>0</v>
@@ -2620,10 +2623,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
@@ -2635,10 +2638,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
@@ -2650,10 +2653,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
         <v>0</v>
@@ -2665,10 +2668,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
@@ -2680,10 +2683,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C85" t="s">
         <v>0</v>
@@ -2695,10 +2698,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
@@ -2710,10 +2713,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
@@ -2725,10 +2728,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
@@ -2740,10 +2743,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
@@ -2755,10 +2758,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
@@ -2770,10 +2773,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
@@ -2785,10 +2788,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C93" t="s">
         <v>0</v>
@@ -2800,10 +2803,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C94" t="s">
         <v>0</v>
@@ -2815,10 +2818,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
@@ -2830,10 +2833,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
@@ -2845,10 +2848,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
@@ -2860,10 +2863,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>62</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C99" t="s">
         <v>0</v>
@@ -2875,10 +2878,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C100" t="s">
         <v>0</v>
@@ -2890,10 +2893,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C101" t="s">
         <v>0</v>
@@ -2905,10 +2908,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>
@@ -2920,10 +2923,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C103" t="s">
         <v>0</v>
@@ -2935,10 +2938,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C104" t="s">
         <v>0</v>
@@ -2950,25 +2953,25 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>72</v>
+        <v>376</v>
       </c>
       <c r="C105" t="s">
         <v>0</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="12"/>
-        <v>part10.Add("its arctic zones ");</v>
+        <v>part10.Add("its lofty peaks ");</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C106" t="s">
         <v>0</v>
@@ -2980,10 +2983,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C107" t="s">
         <v>0</v>
@@ -2995,10 +2998,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C108" t="s">
         <v>0</v>
@@ -3010,10 +3013,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C110" t="s">
         <v>0</v>
@@ -3025,10 +3028,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C111" t="s">
         <v>0</v>
@@ -3040,10 +3043,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C112" t="s">
         <v>0</v>
@@ -3055,10 +3058,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C113" t="s">
         <v>0</v>
@@ -3070,10 +3073,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C114" t="s">
         <v>0</v>
@@ -3085,10 +3088,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C115" t="s">
         <v>0</v>
@@ -3100,10 +3103,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C116" t="s">
         <v>0</v>
@@ -3115,10 +3118,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C117" t="s">
         <v>0</v>
@@ -3130,10 +3133,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C118" t="s">
         <v>0</v>
@@ -3145,10 +3148,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C119" t="s">
         <v>0</v>
@@ -3160,10 +3163,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C121" t="s">
         <v>0</v>
@@ -3175,10 +3178,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
@@ -3190,10 +3193,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>78</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C123" t="s">
         <v>0</v>
@@ -3205,10 +3208,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C124" t="s">
         <v>0</v>
@@ -3220,10 +3223,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C125" t="s">
         <v>0</v>
@@ -3235,10 +3238,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C126" t="s">
         <v>0</v>
@@ -3250,10 +3253,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C127" t="s">
         <v>0</v>
@@ -3265,10 +3268,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C128" t="s">
         <v>0</v>
@@ -3280,10 +3283,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C129" t="s">
         <v>0</v>
@@ -3295,10 +3298,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C130" t="s">
         <v>0</v>
@@ -3310,10 +3313,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C132" t="s">
         <v>0</v>
@@ -3325,10 +3328,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C133" t="s">
         <v>0</v>
@@ -3340,10 +3343,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C134" t="s">
         <v>0</v>
@@ -3355,10 +3358,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C135" t="s">
         <v>0</v>
@@ -3370,10 +3373,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C136" t="s">
         <v>0</v>
@@ -3385,10 +3388,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C137" t="s">
         <v>0</v>
@@ -3400,10 +3403,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C138" t="s">
         <v>0</v>
@@ -3415,10 +3418,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C139" t="s">
         <v>0</v>
@@ -3430,10 +3433,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C140" t="s">
         <v>0</v>
@@ -3445,10 +3448,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C141" t="s">
         <v>0</v>
@@ -3460,10 +3463,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C143" t="s">
         <v>0</v>
@@ -3475,10 +3478,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C144" t="s">
         <v>0</v>
@@ -3490,10 +3493,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C145" t="s">
         <v>0</v>
@@ -3505,10 +3508,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C146" t="s">
         <v>0</v>
@@ -3520,10 +3523,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C147" t="s">
         <v>0</v>
@@ -3535,10 +3538,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C148" t="s">
         <v>0</v>
@@ -3550,10 +3553,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C149" t="s">
         <v>0</v>
@@ -3565,10 +3568,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="C150" t="s">
         <v>0</v>
@@ -3580,10 +3583,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C151" t="s">
         <v>0</v>
@@ -3595,10 +3598,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C152" t="s">
         <v>0</v>
@@ -3610,10 +3613,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C154" t="s">
         <v>0</v>
@@ -3625,10 +3628,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C155" t="s">
         <v>0</v>
@@ -3640,10 +3643,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C156" t="s">
         <v>0</v>
@@ -3655,10 +3658,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C157" t="s">
         <v>0</v>
@@ -3670,10 +3673,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C158" t="s">
         <v>0</v>
@@ -3685,10 +3688,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C159" t="s">
         <v>0</v>
@@ -3700,10 +3703,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C160" t="s">
         <v>0</v>
@@ -3715,10 +3718,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C161" t="s">
         <v>0</v>
@@ -3730,10 +3733,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C162" t="s">
         <v>0</v>
@@ -3745,10 +3748,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C163" t="s">
         <v>0</v>
@@ -3760,10 +3763,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C165" t="s">
         <v>0</v>
@@ -3775,10 +3778,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C166" t="s">
         <v>0</v>
@@ -3790,10 +3793,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C167" t="s">
         <v>0</v>
@@ -3805,10 +3808,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C168" t="s">
         <v>0</v>
@@ -3820,10 +3823,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C169" t="s">
         <v>0</v>
@@ -3835,10 +3838,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C170" t="s">
         <v>0</v>
@@ -3850,10 +3853,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C171" t="s">
         <v>0</v>
@@ -3865,10 +3868,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C172" t="s">
         <v>0</v>
@@ -3880,10 +3883,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C173" t="s">
         <v>0</v>
@@ -3895,10 +3898,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C174" t="s">
         <v>0</v>
@@ -3910,10 +3913,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="C176" t="s">
         <v>0</v>
@@ -3925,10 +3928,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C177" t="s">
         <v>0</v>
@@ -3940,10 +3943,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C178" t="s">
         <v>0</v>
@@ -3955,10 +3958,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C179" t="s">
         <v>0</v>
@@ -3970,10 +3973,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C180" t="s">
         <v>0</v>
@@ -3985,10 +3988,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C181" t="s">
         <v>0</v>
@@ -4000,10 +4003,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C182" t="s">
         <v>0</v>
@@ -4015,10 +4018,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C183" t="s">
         <v>0</v>
@@ -4030,10 +4033,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C184" t="s">
         <v>0</v>
@@ -4045,25 +4048,25 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>219</v>
+        <v>375</v>
       </c>
       <c r="C185" t="s">
         <v>0</v>
       </c>
       <c r="D185" t="str">
         <f t="shared" si="19"/>
-        <v>part17.Add("excreted on by the ");</v>
+        <v>part17.Add("furiously excreted on by the ");</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>111</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C187" t="s">
         <v>0</v>
@@ -4075,10 +4078,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C188" t="s">
         <v>0</v>
@@ -4090,10 +4093,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C189" t="s">
         <v>0</v>
@@ -4105,7 +4108,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" t="s">
@@ -4118,10 +4121,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C191" t="s">
         <v>0</v>
@@ -4133,10 +4136,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C192" t="s">
         <v>0</v>
@@ -4148,10 +4151,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C193" t="s">
         <v>0</v>
@@ -4163,10 +4166,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C194" t="s">
         <v>0</v>
@@ -4178,10 +4181,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C195" t="s">
         <v>0</v>
@@ -4193,10 +4196,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C196" t="s">
         <v>0</v>
@@ -4208,10 +4211,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C198" t="s">
         <v>0</v>
@@ -4223,10 +4226,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C199" t="s">
         <v>0</v>
@@ -4238,10 +4241,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C200" t="s">
         <v>0</v>
@@ -4253,10 +4256,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C201" t="s">
         <v>0</v>
@@ -4268,10 +4271,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C202" t="s">
         <v>0</v>
@@ -4283,10 +4286,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C203" t="s">
         <v>0</v>
@@ -4298,25 +4301,25 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>305</v>
+        <v>374</v>
       </c>
       <c r="C204" t="s">
         <v>0</v>
       </c>
       <c r="D204" t="str">
         <f t="shared" si="21"/>
-        <v>part19.Add("curiously heptagonal ");</v>
+        <v>part19.Add("heptagonally gendered ");</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C205" t="s">
         <v>0</v>
@@ -4328,10 +4331,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C206" t="s">
         <v>0</v>
@@ -4343,10 +4346,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C207" t="s">
         <v>0</v>
@@ -4358,10 +4361,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C209" t="s">
         <v>0</v>
@@ -4373,10 +4376,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C210" t="s">
         <v>0</v>
@@ -4388,10 +4391,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>129</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C211" t="s">
         <v>0</v>
@@ -4403,10 +4406,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C212" t="s">
         <v>0</v>
@@ -4418,10 +4421,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C213" t="s">
         <v>0</v>
@@ -4433,10 +4436,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C214" t="s">
         <v>0</v>
@@ -4448,10 +4451,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C215" t="s">
         <v>0</v>
@@ -4463,10 +4466,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C216" t="s">
         <v>0</v>
@@ -4478,10 +4481,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C217" t="s">
         <v>0</v>
@@ -4493,10 +4496,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C218" t="s">
         <v>0</v>
@@ -4508,10 +4511,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B220" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C220" t="s">
         <v>0</v>
@@ -4523,10 +4526,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B221" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C221" t="s">
         <v>0</v>
@@ -4538,10 +4541,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B222" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C222" t="s">
         <v>0</v>
@@ -4553,10 +4556,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B223" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C223" t="s">
         <v>0</v>
@@ -4568,10 +4571,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B224" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C224" t="s">
         <v>0</v>
@@ -4583,10 +4586,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B225" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C225" t="s">
         <v>0</v>
@@ -4598,10 +4601,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B226" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C226" t="s">
         <v>0</v>
@@ -4613,10 +4616,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B227" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C227" t="s">
         <v>0</v>
@@ -4628,10 +4631,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B228" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C228" t="s">
         <v>0</v>
@@ -4643,10 +4646,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C229" t="s">
         <v>0</v>
@@ -4658,10 +4661,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B231" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C231" t="s">
         <v>0</v>
@@ -4673,10 +4676,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B232" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C232" t="s">
         <v>0</v>
@@ -4688,10 +4691,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B233" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C233" t="s">
         <v>0</v>
@@ -4703,10 +4706,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B234" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C234" t="s">
         <v>0</v>
@@ -4718,10 +4721,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B235" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C235" t="s">
         <v>0</v>
@@ -4733,10 +4736,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B236" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C236" t="s">
         <v>0</v>
@@ -4748,10 +4751,10 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C237" t="s">
         <v>0</v>
@@ -4763,10 +4766,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B238" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C238" t="s">
         <v>0</v>
@@ -4778,10 +4781,10 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B239" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C239" t="s">
         <v>0</v>
@@ -4793,10 +4796,10 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B240" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C240" t="s">
         <v>0</v>
@@ -4808,10 +4811,10 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B242" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C242" t="s">
         <v>0</v>
@@ -4823,10 +4826,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B243" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C243" t="s">
         <v>0</v>
@@ -4838,10 +4841,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B244" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C244" t="s">
         <v>0</v>
@@ -4853,10 +4856,10 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B245" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C245" t="s">
         <v>0</v>
@@ -4868,10 +4871,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B246" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C246" t="s">
         <v>0</v>
@@ -4883,10 +4886,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B247" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C247" t="s">
         <v>0</v>
@@ -4898,10 +4901,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B248" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C248" t="s">
         <v>0</v>
@@ -4913,10 +4916,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B249" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C249" t="s">
         <v>0</v>
@@ -4928,10 +4931,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B250" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C250" t="s">
         <v>0</v>
@@ -4943,10 +4946,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B251" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C251" t="s">
         <v>0</v>
@@ -4958,10 +4961,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B253" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C253" t="s">
         <v>0</v>
@@ -4973,10 +4976,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B254" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C254" t="s">
         <v>0</v>
@@ -4988,10 +4991,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C255" t="s">
         <v>0</v>
@@ -5003,10 +5006,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C256" t="s">
         <v>0</v>
@@ -5018,10 +5021,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C257" t="s">
         <v>0</v>
@@ -5033,10 +5036,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C258" t="s">
         <v>0</v>
@@ -5048,10 +5051,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C259" t="s">
         <v>0</v>
@@ -5063,10 +5066,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C260" t="s">
         <v>0</v>
@@ -5078,10 +5081,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C261" t="s">
         <v>0</v>
@@ -5093,10 +5096,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C262" t="s">
         <v>0</v>
@@ -5108,10 +5111,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B264" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C264" t="s">
         <v>0</v>
@@ -5123,10 +5126,10 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B265" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C265" t="s">
         <v>0</v>
@@ -5138,10 +5141,10 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C266" t="s">
         <v>0</v>
@@ -5153,10 +5156,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C267" t="s">
         <v>0</v>
@@ -5168,10 +5171,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C268" t="s">
         <v>0</v>
@@ -5183,10 +5186,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C269" t="s">
         <v>0</v>
@@ -5198,40 +5201,40 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>320</v>
+        <v>371</v>
       </c>
       <c r="C270" t="s">
         <v>0</v>
       </c>
       <c r="D270" t="str">
         <f t="shared" si="27"/>
-        <v>part25.Add(". These beings are projected to evolve into ");</v>
+        <v>part25.Add(". These curious creatures are being ruthlessly slaughtered towards extinction by a roaming horde of ");</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>321</v>
+        <v>370</v>
       </c>
       <c r="C271" t="s">
         <v>0</v>
       </c>
       <c r="D271" t="str">
         <f t="shared" si="27"/>
-        <v>part25.Add(". In barely comprehensible ways these creatures are pleading to become ");</v>
+        <v>part25.Add(". These beings, who are actually the smartest things on the world, are typically worn as hats by the local, ");</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C272" t="s">
         <v>0</v>
@@ -5243,10 +5246,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C273" t="s">
         <v>0</v>
@@ -5258,10 +5261,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B275" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C275" t="s">
         <v>0</v>
@@ -5273,10 +5276,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B276" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C276" t="s">
         <v>0</v>
@@ -5288,10 +5291,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B277" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C277" t="s">
         <v>0</v>
@@ -5303,10 +5306,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B278" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C278" t="s">
         <v>0</v>
@@ -5318,10 +5321,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B279" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C279" t="s">
         <v>0</v>
@@ -5333,10 +5336,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B280" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C280" t="s">
         <v>0</v>
@@ -5348,10 +5351,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B281" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C281" t="s">
         <v>0</v>
@@ -5363,10 +5366,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B282" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C282" t="s">
         <v>0</v>
@@ -5378,10 +5381,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B283" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C283" t="s">
         <v>0</v>
@@ -5393,10 +5396,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B284" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C284" t="s">
         <v>0</v>
@@ -5408,10 +5411,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B286" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C286" t="s">
         <v>0</v>
@@ -5423,10 +5426,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B287" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C287" t="s">
         <v>0</v>
@@ -5438,10 +5441,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B288" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C288" t="s">
         <v>0</v>
@@ -5453,10 +5456,10 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B289" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C289" t="s">
         <v>0</v>
@@ -5468,10 +5471,10 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B290" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C290" t="s">
         <v>0</v>
@@ -5483,10 +5486,10 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B291" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C291" t="s">
         <v>0</v>
@@ -5498,10 +5501,10 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B292" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C292" t="s">
         <v>0</v>
@@ -5513,10 +5516,10 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B293" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C293" t="s">
         <v>0</v>
@@ -5528,10 +5531,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B294" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C294" t="s">
         <v>0</v>
@@ -5543,10 +5546,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B295" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C295" t="s">
         <v>0</v>
@@ -5558,25 +5561,25 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B297" t="s">
-        <v>242</v>
+        <v>372</v>
       </c>
       <c r="C297" t="s">
         <v>0</v>
       </c>
       <c r="D297" t="str">
         <f>A297&amp;".Add("&amp;C297&amp;B297&amp;C297&amp;");"</f>
-        <v>part28.Add("who seem quite happy to trade us their ");</v>
+        <v>part28.Add("who themselves seem quite happy to trade us their ");</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B298" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C298" t="s">
         <v>0</v>
@@ -5588,10 +5591,10 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B299" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C299" t="s">
         <v>0</v>
@@ -5603,10 +5606,10 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B300" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C300" t="s">
         <v>0</v>
@@ -5618,10 +5621,10 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B301" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C301" t="s">
         <v>0</v>
@@ -5633,10 +5636,10 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B302" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C302" t="s">
         <v>0</v>
@@ -5648,10 +5651,10 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B303" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C303" t="s">
         <v>0</v>
@@ -5663,10 +5666,10 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B304" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C304" t="s">
         <v>0</v>
@@ -5678,10 +5681,10 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B305" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C305" t="s">
         <v>0</v>
@@ -5693,25 +5696,25 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B306" t="s">
-        <v>200</v>
+        <v>373</v>
       </c>
       <c r="C306" t="s">
         <v>0</v>
       </c>
       <c r="D306" t="str">
         <f t="shared" si="30"/>
-        <v>part28.Add("who may be swiftly swindled of their ");</v>
+        <v>part28.Add("who, might I suggest, may be swiftly swindled of their ");</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B308" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C308" t="s">
         <v>0</v>
@@ -5723,10 +5726,10 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B309" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C309" t="s">
         <v>0</v>
@@ -5738,10 +5741,10 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B310" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C310" t="s">
         <v>0</v>
@@ -5753,10 +5756,10 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B311" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C311" t="s">
         <v>0</v>
@@ -5768,10 +5771,10 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B312" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C312" t="s">
         <v>0</v>
@@ -5783,10 +5786,10 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B313" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C313" t="s">
         <v>0</v>
@@ -5798,10 +5801,10 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B314" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C314" t="s">
         <v>0</v>
@@ -5813,10 +5816,10 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B315" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C315" t="s">
         <v>0</v>
@@ -5828,10 +5831,10 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B316" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C316" t="s">
         <v>0</v>
@@ -5843,10 +5846,10 @@
     </row>
     <row r="317" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="C317" t="s">
         <v>0</v>
@@ -5858,10 +5861,10 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
+        <v>165</v>
+      </c>
+      <c r="B319" t="s">
         <v>168</v>
-      </c>
-      <c r="B319" t="s">
-        <v>171</v>
       </c>
       <c r="C319" t="s">
         <v>0</v>
@@ -5873,10 +5876,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B320" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C320" t="s">
         <v>0</v>
@@ -5888,10 +5891,10 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B321" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C321" t="s">
         <v>0</v>
@@ -5903,10 +5906,10 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B322" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C322" t="s">
         <v>0</v>
@@ -5918,10 +5921,10 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B323" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C323" t="s">
         <v>0</v>
@@ -5933,10 +5936,10 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B324" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C324" t="s">
         <v>0</v>
@@ -5948,10 +5951,10 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B325" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C325" t="s">
         <v>0</v>
@@ -5963,10 +5966,10 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B326" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C326" t="s">
         <v>0</v>
@@ -5978,10 +5981,10 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B327" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C327" t="s">
         <v>0</v>
@@ -5993,10 +5996,10 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B328" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C328" t="s">
         <v>0</v>
@@ -6008,10 +6011,10 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B331" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C331" t="s">
         <v>0</v>
@@ -6023,10 +6026,10 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B332" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C332" t="s">
         <v>0</v>
@@ -6038,10 +6041,10 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B333" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C333" t="s">
         <v>0</v>
@@ -6053,25 +6056,25 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B334" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="C334" t="s">
         <v>0</v>
       </c>
       <c r="D334" t="str">
         <f t="shared" si="33"/>
-        <v>part31.Add("foul-smelling but addictive ointment. ");</v>
+        <v>part31.Add("foul-smelling but addictive herbal ointment. ");</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B335" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C335" t="s">
         <v>0</v>
@@ -6083,10 +6086,10 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B336" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C336" t="s">
         <v>0</v>
@@ -6098,10 +6101,10 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B337" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C337" t="s">
         <v>0</v>
@@ -6113,10 +6116,10 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B338" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C338" t="s">
         <v>0</v>
@@ -6128,10 +6131,10 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B339" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C339" t="s">
         <v>0</v>
@@ -6143,10 +6146,10 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B340" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C340" t="s">
         <v>0</v>
@@ -6179,21 +6182,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C2" t="str">
         <f>$A$1&amp;".Add("&amp;E2&amp;A2&amp;E2&amp;");"</f>
@@ -6209,10 +6212,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C11" si="0">$A$1&amp;".Add("&amp;E3&amp;A3&amp;E3&amp;");"</f>
@@ -6228,10 +6231,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -6247,10 +6250,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -6266,10 +6269,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -6285,10 +6288,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -6304,10 +6307,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -6323,10 +6326,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -6342,10 +6345,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -6361,10 +6364,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -6385,10 +6388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6401,10 +6404,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C1" t="str">
         <f t="shared" ref="C1:C10" si="0">B$1&amp;".Add("&amp;D1&amp;A1&amp;D1&amp;");"</f>
@@ -6416,10 +6419,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
@@ -6431,10 +6434,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -6446,10 +6449,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -6461,10 +6464,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -6476,10 +6479,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -6491,10 +6494,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -6506,10 +6509,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -6521,10 +6524,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -6536,10 +6539,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -6551,16 +6554,31 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11" si="1">B$1&amp;".Add("&amp;D11&amp;A11&amp;D11&amp;");"</f>
         <v>cameraFails.Add("Unknown camera issue - sorry about that");</v>
       </c>
       <c r="D11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" ref="C12" si="2">B$1&amp;".Add("&amp;D12&amp;A12&amp;D12&amp;");"</f>
+        <v>cameraFails.Add("Hmm, the camera is not working. Close your eyes and wish upon a star?");</v>
+      </c>
+      <c r="D12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6584,37 +6602,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>